<commit_message>
1.add global dict 2.Delete Console Output Log 3.Modify domestic API use cases
</commit_message>
<xml_diff>
--- a/test_data/hw_test/test_smoke.xlsx
+++ b/test_data/hw_test/test_smoke.xlsx
@@ -15,12 +15,13 @@
     <sheet name="cloud_api_v8_test_data" sheetId="1" r:id="rId1"/>
     <sheet name="api_notv8_test_data" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525" calcOnSave="0" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="144">
   <si>
     <t>项目名称</t>
   </si>
@@ -440,11 +441,6 @@
   </si>
   <si>
     <t>{ 'user_id': '12338806','seq': 1, 'cur_time': '1614581155012'}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v8/cloud/status
-</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Get cloud status of device</t>
@@ -506,12 +502,58 @@
     <t>v8/list</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">v8/cloud/status
+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v8/judge/equipment/active</t>
+  </si>
+  <si>
+    <t>Get cloud free info</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v8/getTrial</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>/orderpay/</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "appPlatform": "yihome",
+  "hmac": "5ePqwD/HmUCs6hNzTSVVqLR3QK8=",
+  "region": "USA",
+  "seq": "1",
+  "userid": "3206905"
+}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get cloud trial</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v8/have/subscription</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>/orderpay/</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query subscription</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,12 +565,14 @@
       <b/>
       <sz val="12"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -558,6 +602,26 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -689,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -732,6 +796,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1036,11 +1114,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H37" sqref="B37:H37"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1117,7 +1195,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="s">
@@ -1255,13 +1333,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="11" t="s">
@@ -1904,7 +1982,7 @@
         <v>13</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I36" s="6" t="s">
         <v>101</v>
@@ -1912,16 +1990,16 @@
     </row>
     <row r="37" spans="1:9" ht="99">
       <c r="A37" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="11" t="s">
@@ -1931,28 +2009,88 @@
         <v>13</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="99">
+      <c r="B38" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="97.5">
+      <c r="B39" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="97.5">
+      <c r="B40" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="25" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 F4 F8 F9 F1:F2 F5:F6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8:F9 F1:F6">
       <formula1>"get,post,put"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3 G4 G8 G9 G10 G11 G12 G13 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25 G26 G27 G28 G29 G30 G31 G32 G33 G34 G35 G36 G37 G1:G2 G5:G7 G14:G15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G40">
       <formula1>"params,data,json"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10 F11 F12 F13 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25 F26 F27 F28 F29 F30 F31 F32 F33 F34 F35 F36 F37 F14:F15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F40">
       <formula1>"get,post,put,delete"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="G1" listDataValidation="1"/>
   </ignoredErrors>

</xml_diff>